<commit_message>
'sincronização, iniciando no quinto'
</commit_message>
<xml_diff>
--- a/resultados/comportamentoMMQ_slot01.xlsx
+++ b/resultados/comportamentoMMQ_slot01.xlsx
@@ -476,7 +476,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>bcspwr02.mtx</t>
+          <t>c130.mtx</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.06973010592100816</v>
+        <v>0.3014476464962595</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -496,10 +496,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.0767783956846045</v>
+        <v>0.001900671329092778</v>
       </c>
       <c r="H2" t="n">
-        <v>6.402570196534391</v>
+        <v>2.210914482212023</v>
       </c>
     </row>
     <row r="3">
@@ -508,7 +508,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>bcspwr02.mtx</t>
+          <t>c130.mtx</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.254434916750539</v>
+        <v>0.5774735832538551</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -528,10 +528,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.963085310254297</v>
+        <v>0.1114351120097399</v>
       </c>
       <c r="H3" t="n">
-        <v>10.24283376604743</v>
+        <v>1.892341904897323</v>
       </c>
     </row>
     <row r="4">
@@ -540,7 +540,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>bcspwr02.mtx</t>
+          <t>c130.mtx</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.06364499088045968</v>
+        <v>0.2718054140736049</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -560,10 +560,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.006121910637598674</v>
+        <v>0.0008801273783611369</v>
       </c>
       <c r="H4" t="n">
-        <v>5.087894619812827</v>
+        <v>2.202644278209048</v>
       </c>
     </row>
     <row r="5">
@@ -572,7 +572,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>bcspwr02.mtx</t>
+          <t>c130.mtx</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -581,7 +581,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.06364499088045968</v>
+        <v>0.2718054140736049</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -592,10 +592,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9938967900765014</v>
+        <v>1.000880514804115</v>
       </c>
       <c r="H5" t="n">
-        <v>5.087894619812827</v>
+        <v>2.202644278209048</v>
       </c>
     </row>
     <row r="6">
@@ -604,7 +604,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>bcspwr02.mtx</t>
+          <t>c130.mtx</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -613,7 +613,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.2403422583072474</v>
+        <v>0.5369101909495564</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -624,10 +624,10 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.1592362303056263</v>
+        <v>0.0523989061570091</v>
       </c>
       <c r="H6" t="n">
-        <v>6.962516785295057</v>
+        <v>1.894693432329337</v>
       </c>
     </row>
     <row r="7">
@@ -636,7 +636,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>bcspwr02.mtx</t>
+          <t>c130.mtx</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -645,7 +645,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.1769798398374348</v>
+        <v>0.5400567740458213</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -653,13 +653,13 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>9.051912444856127</v>
+        <v>2.061218349762739</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.4552558597305666</v>
+        <v>0.008991857049291702</v>
       </c>
       <c r="H7" t="n">
-        <v>0.00923115765965761</v>
+        <v>-6.009479423897384e-05</v>
       </c>
     </row>
     <row r="8">
@@ -668,7 +668,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>bcspwr02.mtx</t>
+          <t>c130.mtx</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.1159311016298055</v>
+        <v>0.235221790856798</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -688,10 +688,10 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.2113230842957536</v>
+        <v>0.01572682349003918</v>
       </c>
       <c r="H8" t="n">
-        <v>7.826055636973508</v>
+        <v>1.905833552772259</v>
       </c>
     </row>
     <row r="9">
@@ -700,7 +700,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>bcspwr02.mtx</t>
+          <t>c130.mtx</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -709,7 +709,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.3349672253352403</v>
+        <v>0.3587297924762985</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -720,10 +720,10 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>-3.058487559335971</v>
+        <v>0.3497527531317776</v>
       </c>
       <c r="H9" t="n">
-        <v>12.16611763768135</v>
+        <v>1.218017422533633</v>
       </c>
     </row>
     <row r="10">
@@ -732,7 +732,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>bcspwr02.mtx</t>
+          <t>c130.mtx</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.1086237258006011</v>
+        <v>0.1898342401085925</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -752,10 +752,10 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.01707504617884745</v>
+        <v>0.00957990274833607</v>
       </c>
       <c r="H10" t="n">
-        <v>5.720880759694117</v>
+        <v>1.790682758708521</v>
       </c>
     </row>
     <row r="11">
@@ -764,7 +764,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>bcspwr02.mtx</t>
+          <t>c130.mtx</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -773,7 +773,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.1086237258006011</v>
+        <v>0.1898342401085925</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -784,10 +784,10 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.9830699062265483</v>
+        <v>1.009625936900139</v>
       </c>
       <c r="H11" t="n">
-        <v>5.720880759694117</v>
+        <v>1.790682758708521</v>
       </c>
     </row>
     <row r="12">
@@ -796,7 +796,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>bcspwr02.mtx</t>
+          <t>c130.mtx</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -805,7 +805,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.3207501036237032</v>
+        <v>0.2912306282251028</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -816,10 +816,10 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.249828248456602</v>
+        <v>0.2136817992765641</v>
       </c>
       <c r="H12" t="n">
-        <v>8.17406962600996</v>
+        <v>1.175566150587699</v>
       </c>
     </row>
     <row r="13">
@@ -828,7 +828,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>bcspwr02.mtx</t>
+          <t>c130.mtx</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -837,7 +837,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.2817953844193738</v>
+        <v>0.4074450231749622</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -845,13 +845,13 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>12.26043779564055</v>
+        <v>1.336063964487185</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.234642043988147</v>
+        <v>0.08135473418256069</v>
       </c>
       <c r="H13" t="n">
-        <v>0.04093275838769575</v>
+        <v>-0.001491543424830034</v>
       </c>
     </row>
     <row r="14">
@@ -869,7 +869,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.0887165081740658</v>
+        <v>0.5720778474031821</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -880,10 +880,10 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.6285097850212445</v>
+        <v>0.01436741027597316</v>
       </c>
       <c r="H14" t="n">
-        <v>23.05644462205588</v>
+        <v>9.779989365251804</v>
       </c>
     </row>
     <row r="15">
@@ -901,7 +901,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.2894481964176644</v>
+        <v>0.7778377964466013</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -912,10 +912,10 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>-11.7518016319687</v>
+        <v>0.2485614021561271</v>
       </c>
       <c r="H15" t="n">
-        <v>42.56016907969617</v>
+        <v>9.348064645344037</v>
       </c>
     </row>
     <row r="16">
@@ -933,7 +933,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.06372652303670007</v>
+        <v>0.5671794233869915</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -944,10 +944,10 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.01272323009088832</v>
+        <v>0.001447988807359192</v>
       </c>
       <c r="H16" t="n">
-        <v>13.09361027500226</v>
+        <v>9.779411920889467</v>
       </c>
     </row>
     <row r="17">
@@ -965,7 +965,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.06372652303670007</v>
+        <v>0.5671794233869915</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -976,10 +976,10 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0.9873573680162143</v>
+        <v>1.001449037649328</v>
       </c>
       <c r="H17" t="n">
-        <v>13.09361027500226</v>
+        <v>9.779411920889467</v>
       </c>
     </row>
     <row r="18">
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.2367873414520035</v>
+        <v>0.7732960432757605</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1008,10 +1008,10 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.253878377844421</v>
+        <v>0.02508511557069801</v>
       </c>
       <c r="H18" t="n">
-        <v>20.22092604008433</v>
+        <v>9.361955671302583</v>
       </c>
     </row>
     <row r="19">
@@ -1029,7 +1029,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.2234631786129274</v>
+        <v>0.8897809263018618</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1037,13 +1037,13 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>39.62638292194563</v>
+        <v>9.380079017512774</v>
       </c>
       <c r="G19" t="n">
-        <v>-3.735373216250576</v>
+        <v>0.07035485895943812</v>
       </c>
       <c r="H19" t="n">
-        <v>0.1002214010073978</v>
+        <v>-0.001599641390956145</v>
       </c>
     </row>
     <row r="20">
@@ -1061,7 +1061,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.1778203034957667</v>
+        <v>0.1890405202025181</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1072,10 +1072,10 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>-2.477920159284486</v>
+        <v>0.006913888386080837</v>
       </c>
       <c r="H20" t="n">
-        <v>36.49618654636986</v>
+        <v>10.03525791890815</v>
       </c>
     </row>
     <row r="21">
@@ -1093,7 +1093,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.4177894505197198</v>
+        <v>0.2899339121870907</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1104,10 +1104,10 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>-21.72194395619105</v>
+        <v>0.07922810333931926</v>
       </c>
       <c r="H21" t="n">
-        <v>57.07458589998441</v>
+        <v>9.926340877405144</v>
       </c>
     </row>
     <row r="22">
@@ -1125,7 +1125,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.1458639901049008</v>
+        <v>0.1896935971724181</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1136,10 +1136,10 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.05364566787580034</v>
+        <v>0.0006898653378037816</v>
       </c>
       <c r="H22" t="n">
-        <v>17.83262874242278</v>
+        <v>10.03480462129615</v>
       </c>
     </row>
     <row r="23">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.1458639901049008</v>
+        <v>0.1896935971724181</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1168,10 +1168,10 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>0.9477678716153</v>
+        <v>1.000690103349625</v>
       </c>
       <c r="H23" t="n">
-        <v>17.83262874242278</v>
+        <v>10.03480462129615</v>
       </c>
     </row>
     <row r="24">
@@ -1189,7 +1189,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.3658129458798124</v>
+        <v>0.2906495636960259</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1200,10 +1200,10 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.4858625955595237</v>
+        <v>0.007901465808541022</v>
       </c>
       <c r="H24" t="n">
-        <v>28.66123001407777</v>
+        <v>9.92642648313832</v>
       </c>
     </row>
     <row r="25">
@@ -1221,7 +1221,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.4107042209120779</v>
+        <v>0.5617220026690884</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1229,13 +1229,13 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>69.98760416282205</v>
+        <v>9.722427462943804</v>
       </c>
       <c r="G25" t="n">
-        <v>-14.29842049450292</v>
+        <v>0.07643176748926699</v>
       </c>
       <c r="H25" t="n">
-        <v>0.7387812709511522</v>
+        <v>-0.003475893955159363</v>
       </c>
     </row>
     <row r="26">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>38_bus.mtx</t>
+          <t>bcspwr02.mtx</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1253,7 +1253,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.6298706669486681</v>
+        <v>0.6322779780930941</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1264,10 +1264,10 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>1497.975426177219</v>
+        <v>0.0009096346051066049</v>
       </c>
       <c r="H26" t="n">
-        <v>5400.861865821704</v>
+        <v>4.279697576607647</v>
       </c>
     </row>
     <row r="27">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>38_bus.mtx</t>
+          <t>bcspwr02.mtx</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1285,7 +1285,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.7724830471756003</v>
+        <v>0.8479589341570655</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1296,10 +1296,10 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>13102.38016598089</v>
+        <v>0.01933607225537032</v>
       </c>
       <c r="H27" t="n">
-        <v>-6240.050058865218</v>
+        <v>4.242616666825635</v>
       </c>
     </row>
     <row r="28">
@@ -1308,7 +1308,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>38_bus.mtx</t>
+          <t>bcspwr02.mtx</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.5858252677102456</v>
+        <v>0.6310283928431806</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1328,10 +1328,10 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>0.1496984629494328</v>
+        <v>0.0002119307191046144</v>
       </c>
       <c r="H28" t="n">
-        <v>2608.170173240099</v>
+        <v>4.279691680208774</v>
       </c>
     </row>
     <row r="29">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>38_bus.mtx</t>
+          <t>bcspwr02.mtx</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1349,7 +1349,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.5858252677102456</v>
+        <v>0.6310283928431806</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1360,10 +1360,10 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>1.161483959471827</v>
+        <v>1.000211953178006</v>
       </c>
       <c r="H29" t="n">
-        <v>2608.170173240099</v>
+        <v>4.279691680208774</v>
       </c>
     </row>
     <row r="30">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>38_bus.mtx</t>
+          <t>bcspwr02.mtx</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1381,7 +1381,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.7582582670608088</v>
+        <v>0.8469268337746113</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1392,10 +1392,10 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>1.345143412116899</v>
+        <v>0.00450671725874573</v>
       </c>
       <c r="H30" t="n">
-        <v>753.1532720549865</v>
+        <v>4.242855866031287</v>
       </c>
     </row>
     <row r="31">
@@ -1404,7 +1404,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>38_bus.mtx</t>
+          <t>bcspwr02.mtx</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1413,7 +1413,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.8643705103035273</v>
+        <v>0.8990316520422359</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1421,13 +1421,13 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>-9464.076530876053</v>
+        <v>4.25433874884664</v>
       </c>
       <c r="G31" t="n">
-        <v>5214.210025351656</v>
+        <v>0.003774439414927322</v>
       </c>
       <c r="H31" t="n">
-        <v>-161.5754173554103</v>
+        <v>-6.366232910712369e-05</v>
       </c>
     </row>
     <row r="32">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>38_bus.mtx</t>
+          <t>bcspwr02.mtx</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1445,7 +1445,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.4258435751075086</v>
+        <v>0.63122982753024</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1456,10 +1456,10 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>3168.596369128384</v>
+        <v>0.001102254860111555</v>
       </c>
       <c r="H32" t="n">
-        <v>-10826.61345021836</v>
+        <v>4.287229411596624</v>
       </c>
     </row>
     <row r="33">
@@ -1468,7 +1468,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>38_bus.mtx</t>
+          <t>bcspwr02.mtx</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1477,7 +1477,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.2928683750315726</v>
+        <v>0.8078739068160115</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1488,10 +1488,10 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>14200.29841021894</v>
+        <v>0.01578868242588802</v>
       </c>
       <c r="H33" t="n">
-        <v>-12613.77340409247</v>
+        <v>4.2624720364885</v>
       </c>
     </row>
     <row r="34">
@@ -1500,7 +1500,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>38_bus.mtx</t>
+          <t>bcspwr02.mtx</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1508,7 +1508,9 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr"/>
+      <c r="D34" t="n">
+        <v>0.6305580519839665</v>
+      </c>
       <c r="E34" t="inlineStr">
         <is>
           <t>Exponencial</t>
@@ -1517,8 +1519,12 @@
       <c r="F34" t="n">
         <v>0</v>
       </c>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
+      <c r="G34" t="n">
+        <v>0.0002564655251213357</v>
+      </c>
+      <c r="H34" t="n">
+        <v>4.28723182843493</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1526,7 +1532,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>38_bus.mtx</t>
+          <t>bcspwr02.mtx</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1534,7 +1540,9 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr"/>
+      <c r="D35" t="n">
+        <v>0.6305580519839665</v>
+      </c>
       <c r="E35" t="inlineStr">
         <is>
           <t>Geometrico</t>
@@ -1543,8 +1551,12 @@
       <c r="F35" t="n">
         <v>0</v>
       </c>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
+      <c r="G35" t="n">
+        <v>1.000256498415216</v>
+      </c>
+      <c r="H35" t="n">
+        <v>4.28723182843493</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1552,7 +1564,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>38_bus.mtx</t>
+          <t>bcspwr02.mtx</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1560,7 +1572,9 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr"/>
+      <c r="D36" t="n">
+        <v>0.8072802199029957</v>
+      </c>
       <c r="E36" t="inlineStr">
         <is>
           <t>Potencial</t>
@@ -1569,8 +1583,12 @@
       <c r="F36" t="n">
         <v>0</v>
       </c>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
+      <c r="G36" t="n">
+        <v>0.003674213974027938</v>
+      </c>
+      <c r="H36" t="n">
+        <v>4.26260005189775</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1578,7 +1596,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>38_bus.mtx</t>
+          <t>bcspwr02.mtx</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1587,7 +1605,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.4520346270928044</v>
+        <v>0.9159912807330062</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1595,13 +1613,13 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>-2040.974568353883</v>
+        <v>4.261725889045047</v>
       </c>
       <c r="G37" t="n">
-        <v>-126.0182115707951</v>
+        <v>0.005280798103025248</v>
       </c>
       <c r="H37" t="n">
-        <v>219.640972046612</v>
+        <v>-0.0001440876980315143</v>
       </c>
     </row>
     <row r="38">
@@ -1610,7 +1628,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>494_bus.mtx</t>
+          <t>bcspwr03.mtx</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1619,7 +1637,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.6018927641938575</v>
+        <v>0.5661327260170664</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1630,10 +1648,10 @@
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>6.695065689469629</v>
+        <v>0.002459429307348725</v>
       </c>
       <c r="H38" t="n">
-        <v>2198.638882724134</v>
+        <v>5.03837149659054</v>
       </c>
     </row>
     <row r="39">
@@ -1642,7 +1660,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>494_bus.mtx</t>
+          <t>bcspwr03.mtx</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1651,7 +1669,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.7779557911002878</v>
+        <v>0.7855755073310073</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1662,10 +1680,10 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>16.34562534291317</v>
+        <v>0.04812147680348619</v>
       </c>
       <c r="H39" t="n">
-        <v>2202.38972764019</v>
+        <v>4.949469882950509</v>
       </c>
     </row>
     <row r="40">
@@ -1674,7 +1692,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>494_bus.mtx</t>
+          <t>bcspwr03.mtx</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1683,7 +1701,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.6018832635013542</v>
+        <v>0.5640340419231592</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1694,10 +1712,10 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>0.003029708962446876</v>
+        <v>0.0004855670403522726</v>
       </c>
       <c r="H40" t="n">
-        <v>2198.639147405977</v>
+        <v>5.038308290617511</v>
       </c>
     </row>
     <row r="41">
@@ -1706,7 +1724,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>494_bus.mtx</t>
+          <t>bcspwr03.mtx</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1715,7 +1733,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.6018832635013542</v>
+        <v>0.5640340419231592</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1726,10 +1744,10 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>1.003034303169177</v>
+        <v>1.000485684947111</v>
       </c>
       <c r="H41" t="n">
-        <v>2198.639147405977</v>
+        <v>5.038308290617511</v>
       </c>
     </row>
     <row r="42">
@@ -1738,7 +1756,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>494_bus.mtx</t>
+          <t>bcspwr03.mtx</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1747,7 +1765,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.7779474809839555</v>
+        <v>0.7836494223360504</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1758,10 +1776,10 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>0.00739688245736143</v>
+        <v>0.009506643683054435</v>
       </c>
       <c r="H42" t="n">
-        <v>2202.374175940339</v>
+        <v>4.95056288966079</v>
       </c>
     </row>
     <row r="43">
@@ -1770,7 +1788,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>494_bus.mtx</t>
+          <t>bcspwr03.mtx</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1779,7 +1797,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.9339736268764869</v>
+        <v>0.8799366045090343</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1787,13 +1805,13 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>2170.839047840293</v>
+        <v>4.965014083781908</v>
       </c>
       <c r="G43" t="n">
-        <v>34.49490057331206</v>
+        <v>0.01162910590842755</v>
       </c>
       <c r="H43" t="n">
-        <v>-5.559966976768449</v>
+        <v>-0.0002292419150269651</v>
       </c>
     </row>
     <row r="44">
@@ -1802,7 +1820,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>494_bus.mtx</t>
+          <t>bcspwr03.mtx</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1811,7 +1829,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.6020032342478927</v>
+        <v>0.6392362323188753</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1822,10 +1840,10 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>6.695989839016693</v>
+        <v>0.006395677773860937</v>
       </c>
       <c r="H44" t="n">
-        <v>2198.63734247489</v>
+        <v>5.04295252042292</v>
       </c>
     </row>
     <row r="45">
@@ -1834,7 +1852,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>494_bus.mtx</t>
+          <t>bcspwr03.mtx</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1843,7 +1861,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.7780438534619295</v>
+        <v>0.7389301777904742</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1854,10 +1872,10 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>16.34730673710231</v>
+        <v>0.05257948002149621</v>
       </c>
       <c r="H45" t="n">
-        <v>2202.389161874502</v>
+        <v>4.986523395780652</v>
       </c>
     </row>
     <row r="46">
@@ -1866,7 +1884,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>494_bus.mtx</t>
+          <t>bcspwr03.mtx</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1875,7 +1893,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.6019931780293863</v>
+        <v>0.6385202343682935</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1886,10 +1904,10 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>0.003030125064319122</v>
+        <v>0.00125795729842053</v>
       </c>
       <c r="H46" t="n">
-        <v>2198.637622643398</v>
+        <v>5.0430846207929</v>
       </c>
     </row>
     <row r="47">
@@ -1898,7 +1916,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>494_bus.mtx</t>
+          <t>bcspwr03.mtx</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1907,7 +1925,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.6019931780293863</v>
+        <v>0.6385202343682935</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1918,10 +1936,10 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>1.003034720533715</v>
+        <v>1.001258748858584</v>
       </c>
       <c r="H47" t="n">
-        <v>2198.637622643398</v>
+        <v>5.0430846207929</v>
       </c>
     </row>
     <row r="48">
@@ -1930,7 +1948,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>494_bus.mtx</t>
+          <t>bcspwr03.mtx</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1939,7 +1957,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.7780351013085632</v>
+        <v>0.7382403046795525</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1950,10 +1968,10 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>0.007397639511536048</v>
+        <v>0.0103427527960825</v>
       </c>
       <c r="H48" t="n">
-        <v>2202.373614911648</v>
+        <v>4.987411205170424</v>
       </c>
     </row>
     <row r="49">
@@ -1962,7 +1980,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>494_bus.mtx</t>
+          <t>bcspwr03.mtx</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1971,7 +1989,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.9339613915017838</v>
+        <v>0.9395980911731771</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1979,13 +1997,13 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>2170.841358214152</v>
+        <v>4.891083602620155</v>
       </c>
       <c r="G49" t="n">
-        <v>34.49197409975453</v>
+        <v>0.0468940558545991</v>
       </c>
       <c r="H49" t="n">
-        <v>-5.559196852147568</v>
+        <v>-0.002531148630046152</v>
       </c>
     </row>
     <row r="50">
@@ -1994,7 +2012,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>685_bus.mtx</t>
+          <t>38_bus.mtx</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2003,7 +2021,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.6015217668739167</v>
+        <v>0.3341681883441914</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -2014,10 +2032,10 @@
         <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>78.90236213227035</v>
+        <v>816.4295912089219</v>
       </c>
       <c r="H50" t="n">
-        <v>25923.39502979624</v>
+        <v>16307.16117491895</v>
       </c>
     </row>
     <row r="51">
@@ -2026,7 +2044,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>685_bus.mtx</t>
+          <t>38_bus.mtx</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2035,7 +2053,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.7776588449051246</v>
+        <v>0.4922910835077088</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -2046,10 +2064,10 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>192.6582846545935</v>
+        <v>11813.91037263978</v>
       </c>
       <c r="H51" t="n">
-        <v>25967.5813352532</v>
+        <v>-2398.20317906024</v>
       </c>
     </row>
     <row r="52">
@@ -2058,7 +2076,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>685_bus.mtx</t>
+          <t>38_bus.mtx</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2067,7 +2085,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0.6015141313314027</v>
+        <v>0.2531171117151889</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2078,10 +2096,10 @@
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>0.003028308641870581</v>
+        <v>0.06523391680336348</v>
       </c>
       <c r="H52" t="n">
-        <v>25923.39753783861</v>
+        <v>10067.39069245114</v>
       </c>
     </row>
     <row r="53">
@@ -2090,7 +2108,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>685_bus.mtx</t>
+          <t>38_bus.mtx</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2099,7 +2117,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0.6015141313314027</v>
+        <v>0.2531171117151889</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -2110,10 +2128,10 @@
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>1.003032898600587</v>
+        <v>1.067408680010042</v>
       </c>
       <c r="H53" t="n">
-        <v>25923.39753783861</v>
+        <v>10067.39069245114</v>
       </c>
     </row>
     <row r="54">
@@ -2122,7 +2140,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>685_bus.mtx</t>
+          <t>38_bus.mtx</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2131,7 +2149,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.7776520253984075</v>
+        <v>0.3890985729024812</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -2142,10 +2160,10 @@
         <v>0</v>
       </c>
       <c r="G54" t="n">
-        <v>0.007394327335801349</v>
+        <v>0.964248613408507</v>
       </c>
       <c r="H54" t="n">
-        <v>25967.39778302169</v>
+        <v>2146.06352133006</v>
       </c>
     </row>
     <row r="55">
@@ -2154,7 +2172,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>685_bus.mtx</t>
+          <t>38_bus.mtx</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2163,7 +2181,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.9340083114870938</v>
+        <v>0.6643655709381344</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -2171,13 +2189,13 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>25595.46863123709</v>
+        <v>-10986.28033683331</v>
       </c>
       <c r="G55" t="n">
-        <v>406.8287606913985</v>
+        <v>5560.568566427659</v>
       </c>
       <c r="H55" t="n">
-        <v>-65.58527971182551</v>
+        <v>-175.7088509340272</v>
       </c>
     </row>
     <row r="56">
@@ -2186,7 +2204,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>685_bus.mtx</t>
+          <t>38_bus.mtx</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2195,7 +2213,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0.6015217670531006</v>
+        <v>0.4186199725465815</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -2206,10 +2224,10 @@
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>78.90236214993638</v>
+        <v>4845.637502583222</v>
       </c>
       <c r="H56" t="n">
-        <v>25923.39502976679</v>
+        <v>-28509.00578629602</v>
       </c>
     </row>
     <row r="57">
@@ -2218,7 +2236,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>685_bus.mtx</t>
+          <t>38_bus.mtx</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2227,7 +2245,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.777658845048175</v>
+        <v>0.4365456273765832</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -2238,10 +2256,10 @@
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>192.6582846867519</v>
+        <v>43834.26161157045</v>
       </c>
       <c r="H57" t="n">
-        <v>25967.58133524238</v>
+        <v>-78968.54317415322</v>
       </c>
     </row>
     <row r="58">
@@ -2250,7 +2268,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>685_bus.mtx</t>
+          <t>38_bus.mtx</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2258,9 +2276,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D58" t="n">
-        <v>0.6015141315126347</v>
-      </c>
+      <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr">
         <is>
           <t>Exponencial</t>
@@ -2269,12 +2285,8 @@
       <c r="F58" t="n">
         <v>0</v>
       </c>
-      <c r="G58" t="n">
-        <v>0.003028308642552702</v>
-      </c>
-      <c r="H58" t="n">
-        <v>25923.397537809</v>
-      </c>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2282,7 +2294,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>685_bus.mtx</t>
+          <t>38_bus.mtx</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2290,9 +2302,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D59" t="n">
-        <v>0.6015141315126347</v>
-      </c>
+      <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
         <is>
           <t>Geometrico</t>
@@ -2301,12 +2311,8 @@
       <c r="F59" t="n">
         <v>0</v>
       </c>
-      <c r="G59" t="n">
-        <v>1.003032898601271</v>
-      </c>
-      <c r="H59" t="n">
-        <v>25923.397537809</v>
-      </c>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -2314,7 +2320,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>685_bus.mtx</t>
+          <t>38_bus.mtx</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2322,9 +2328,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D60" t="n">
-        <v>0.7776520255416192</v>
-      </c>
+      <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
         <is>
           <t>Potencial</t>
@@ -2333,12 +2337,8 @@
       <c r="F60" t="n">
         <v>0</v>
       </c>
-      <c r="G60" t="n">
-        <v>0.007394327337033419</v>
-      </c>
-      <c r="H60" t="n">
-        <v>25967.39778301089</v>
-      </c>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>685_bus.mtx</t>
+          <t>38_bus.mtx</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2355,7 +2355,7 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0.934008311467092</v>
+        <v>0.4597729810221919</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -2363,13 +2363,13 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>25595.46863128133</v>
+        <v>-77754.39901128554</v>
       </c>
       <c r="G61" t="n">
-        <v>406.8287606353816</v>
+        <v>16256.15544495885</v>
       </c>
       <c r="H61" t="n">
-        <v>-65.58527969708803</v>
+        <v>-600.5535759145066</v>
       </c>
     </row>
     <row r="62">
@@ -2378,7 +2378,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>c130.mtx</t>
+          <t>685_bus.mtx</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2386,9 +2386,7 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D62" t="n">
-        <v>0.02631565975524347</v>
-      </c>
+      <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr">
         <is>
           <t>Linear</t>
@@ -2397,12 +2395,8 @@
       <c r="F62" t="n">
         <v>0</v>
       </c>
-      <c r="G62" t="n">
-        <v>-993.2649435992074</v>
-      </c>
-      <c r="H62" t="n">
-        <v>75490.49057075396</v>
-      </c>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2410,7 +2404,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>c130.mtx</t>
+          <t>685_bus.mtx</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2418,9 +2412,7 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D63" t="n">
-        <v>0.1458653223764264</v>
-      </c>
+      <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr">
         <is>
           <t>Logaritmo</t>
@@ -2429,12 +2421,8 @@
       <c r="F63" t="n">
         <v>0</v>
       </c>
-      <c r="G63" t="n">
-        <v>-82075.49552811417</v>
-      </c>
-      <c r="H63" t="n">
-        <v>327186.407065972</v>
-      </c>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2442,7 +2430,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>c130.mtx</t>
+          <t>685_bus.mtx</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2450,9 +2438,7 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D64" t="n">
-        <v>0.01755298412525413</v>
-      </c>
+      <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
           <t>Exponencial</t>
@@ -2461,12 +2447,8 @@
       <c r="F64" t="n">
         <v>0</v>
       </c>
-      <c r="G64" t="n">
-        <v>-0.00523429693570727</v>
-      </c>
-      <c r="H64" t="n">
-        <v>3.50464768288825</v>
-      </c>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2474,7 +2456,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>c130.mtx</t>
+          <t>685_bus.mtx</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2482,9 +2464,7 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D65" t="n">
-        <v>0.01755298412525413</v>
-      </c>
+      <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
         <is>
           <t>Geometrico</t>
@@ -2493,12 +2473,8 @@
       <c r="F65" t="n">
         <v>0</v>
       </c>
-      <c r="G65" t="n">
-        <v>0.9947793781263162</v>
-      </c>
-      <c r="H65" t="n">
-        <v>3.50464768288825</v>
-      </c>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -2506,7 +2482,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>c130.mtx</t>
+          <t>685_bus.mtx</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2514,9 +2490,7 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D66" t="n">
-        <v>0.117004259192405</v>
-      </c>
+      <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr">
         <is>
           <t>Potencial</t>
@@ -2525,12 +2499,8 @@
       <c r="F66" t="n">
         <v>0</v>
       </c>
-      <c r="G66" t="n">
-        <v>-0.4743110260531581</v>
-      </c>
-      <c r="H66" t="n">
-        <v>15.44766670359824</v>
-      </c>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2538,7 +2508,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>c130.mtx</t>
+          <t>685_bus.mtx</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2546,22 +2516,30 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D67" t="n">
-        <v>0.0686496152788858</v>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
           <t>Polinomial</t>
         </is>
       </c>
-      <c r="F67" t="n">
-        <v>169850.7360987344</v>
-      </c>
-      <c r="G67" t="n">
-        <v>-5916.408188537316</v>
-      </c>
-      <c r="H67" t="n">
-        <v>43.1854670608606</v>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
       </c>
     </row>
     <row r="68">
@@ -2570,7 +2548,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>c130.mtx</t>
+          <t>685_bus.mtx</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2578,9 +2556,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D68" t="n">
-        <v>0.07499970012433577</v>
-      </c>
+      <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr">
         <is>
           <t>Linear</t>
@@ -2589,12 +2565,8 @@
       <c r="F68" t="n">
         <v>0</v>
       </c>
-      <c r="G68" t="n">
-        <v>-8202.080466665326</v>
-      </c>
-      <c r="H68" t="n">
-        <v>218724.4686705104</v>
-      </c>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2602,7 +2574,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>c130.mtx</t>
+          <t>685_bus.mtx</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2610,9 +2582,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D69" t="n">
-        <v>0.2658350775172474</v>
-      </c>
+      <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr">
         <is>
           <t>Logaritmo</t>
@@ -2621,12 +2591,8 @@
       <c r="F69" t="n">
         <v>0</v>
       </c>
-      <c r="G69" t="n">
-        <v>-202026.3450432626</v>
-      </c>
-      <c r="H69" t="n">
-        <v>607052.7257727735</v>
-      </c>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -2634,7 +2600,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>c130.mtx</t>
+          <t>685_bus.mtx</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2642,9 +2608,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D70" t="n">
-        <v>0.05039896675779034</v>
-      </c>
+      <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr">
         <is>
           <t>Exponencial</t>
@@ -2653,12 +2617,8 @@
       <c r="F70" t="n">
         <v>0</v>
       </c>
-      <c r="G70" t="n">
-        <v>-0.04372909698972467</v>
-      </c>
-      <c r="H70" t="n">
-        <v>7.413475728139034</v>
-      </c>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2666,7 +2626,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>c130.mtx</t>
+          <t>685_bus.mtx</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2674,9 +2634,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D71" t="n">
-        <v>0.05039896675779034</v>
-      </c>
+      <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr">
         <is>
           <t>Geometrico</t>
@@ -2685,12 +2643,8 @@
       <c r="F71" t="n">
         <v>0</v>
       </c>
-      <c r="G71" t="n">
-        <v>0.9572132342986717</v>
-      </c>
-      <c r="H71" t="n">
-        <v>7.413475728139034</v>
-      </c>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2698,7 +2652,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>c130.mtx</t>
+          <t>685_bus.mtx</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2706,9 +2660,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D72" t="n">
-        <v>0.2170246399112702</v>
-      </c>
+      <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr">
         <is>
           <t>Potencial</t>
@@ -2717,12 +2669,8 @@
       <c r="F72" t="n">
         <v>0</v>
       </c>
-      <c r="G72" t="n">
-        <v>-1.187194337097301</v>
-      </c>
-      <c r="H72" t="n">
-        <v>79.41459072871872</v>
-      </c>
+      <c r="G72" t="inlineStr"/>
+      <c r="H72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -2730,7 +2678,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>c130.mtx</t>
+          <t>685_bus.mtx</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2738,22 +2686,30 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D73" t="n">
-        <v>0.187804381773135</v>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
           <t>Polinomial</t>
         </is>
       </c>
-      <c r="F73" t="n">
-        <v>492127.4594673469</v>
-      </c>
-      <c r="G73" t="n">
-        <v>-48212.27424181209</v>
-      </c>
-      <c r="H73" t="n">
-        <v>1000.254844378669</v>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
       </c>
     </row>
     <row r="74">
@@ -2762,7 +2718,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>662_bus.mtx</t>
+          <t>h292.mtx</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2771,7 +2727,7 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0.602755815332127</v>
+        <v>0.611769822351</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2782,10 +2738,10 @@
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>4.302909471044041</v>
+        <v>0.009265901587170481</v>
       </c>
       <c r="H74" t="n">
-        <v>1408.643353832635</v>
+        <v>8.833158219804019</v>
       </c>
     </row>
     <row r="75">
@@ -2794,7 +2750,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>662_bus.mtx</t>
+          <t>h292.mtx</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2803,7 +2759,7 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>0.7787603710759297</v>
+        <v>0.8453299634865006</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2814,10 +2770,10 @@
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>10.50321428825977</v>
+        <v>0.2186956882985222</v>
       </c>
       <c r="H75" t="n">
-        <v>1411.055682410303</v>
+        <v>8.393005250382261</v>
       </c>
     </row>
     <row r="76">
@@ -2826,7 +2782,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>662_bus.mtx</t>
+          <t>h292.mtx</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2835,7 +2791,7 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>0.6027419671535538</v>
+        <v>0.6062920878417107</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2846,10 +2802,10 @@
         <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>0.003039148324995722</v>
+        <v>0.001033525498328538</v>
       </c>
       <c r="H76" t="n">
-        <v>1408.643602058284</v>
+        <v>8.832509929952096</v>
       </c>
     </row>
     <row r="77">
@@ -2858,7 +2814,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>662_bus.mtx</t>
+          <t>h292.mtx</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2867,7 +2823,7 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0.6027419671535538</v>
+        <v>0.6062920878417107</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2878,10 +2834,10 @@
         <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>1.0030437712183</v>
+        <v>1.001034059769852</v>
       </c>
       <c r="H77" t="n">
-        <v>1408.643602058284</v>
+        <v>8.832509929952096</v>
       </c>
     </row>
     <row r="78">
@@ -2890,7 +2846,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>662_bus.mtx</t>
+          <t>h292.mtx</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2899,7 +2855,7 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0.7787480179751753</v>
+        <v>0.8409696229780652</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2910,10 +2866,10 @@
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>0.007418454848512015</v>
+        <v>0.02444014795256053</v>
       </c>
       <c r="H78" t="n">
-        <v>1411.045706925363</v>
+        <v>8.408144973066667</v>
       </c>
     </row>
     <row r="79">
@@ -2922,7 +2878,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>662_bus.mtx</t>
+          <t>h292.mtx</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2931,7 +2887,7 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0.9345544053630863</v>
+        <v>0.9135697876643967</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2939,13 +2895,13 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>1390.796823953478</v>
+        <v>8.534637769680124</v>
       </c>
       <c r="G79" t="n">
-        <v>22.149439350201</v>
+        <v>0.04004120572365471</v>
       </c>
       <c r="H79" t="n">
-        <v>-3.569305975831369</v>
+        <v>-0.0006155060827296841</v>
       </c>
     </row>
     <row r="80">
@@ -2954,7 +2910,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>662_bus.mtx</t>
+          <t>h292.mtx</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2963,7 +2919,7 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>0.6027558153850775</v>
+        <v>0.2095217890593369</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2974,10 +2930,10 @@
         <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>4.302909471328166</v>
+        <v>0.003603156050796159</v>
       </c>
       <c r="H80" t="n">
-        <v>1408.643353832161</v>
+        <v>9.09306595001212</v>
       </c>
     </row>
     <row r="81">
@@ -2986,7 +2942,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>662_bus.mtx</t>
+          <t>h292.mtx</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2995,7 +2951,7 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0.7787603711179606</v>
+        <v>0.360552783264742</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3006,10 +2962,10 @@
         <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>10.50321428877567</v>
+        <v>0.05810352859530711</v>
       </c>
       <c r="H81" t="n">
-        <v>1411.055682410128</v>
+        <v>8.995411513252145</v>
       </c>
     </row>
     <row r="82">
@@ -3018,7 +2974,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>662_bus.mtx</t>
+          <t>h292.mtx</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3027,7 +2983,7 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>0.6027419672059002</v>
+        <v>0.2098006284487261</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -3038,10 +2994,10 @@
         <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>0.003039148325194674</v>
+        <v>0.0003970311420511488</v>
       </c>
       <c r="H82" t="n">
-        <v>1408.64360205782</v>
+        <v>9.092725495255012</v>
       </c>
     </row>
     <row r="83">
@@ -3050,7 +3006,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>662_bus.mtx</t>
+          <t>h292.mtx</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3059,7 +3015,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>0.6027419672059002</v>
+        <v>0.2098006284487261</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3070,10 +3026,10 @@
         <v>0</v>
       </c>
       <c r="G83" t="n">
-        <v>1.003043771218499</v>
+        <v>1.000397109969347</v>
       </c>
       <c r="H83" t="n">
-        <v>1408.64360205782</v>
+        <v>9.092725495255012</v>
       </c>
     </row>
     <row r="84">
@@ -3082,7 +3038,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>662_bus.mtx</t>
+          <t>h292.mtx</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3091,7 +3047,7 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>0.7787480180164593</v>
+        <v>0.3607611824426773</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -3102,10 +3058,10 @@
         <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>0.007418454848872461</v>
+        <v>0.006400010525037557</v>
       </c>
       <c r="H84" t="n">
-        <v>1411.045706925202</v>
+        <v>8.99546271980766</v>
       </c>
     </row>
     <row r="85">
@@ -3114,7 +3070,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>662_bus.mtx</t>
+          <t>h292.mtx</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3123,7 +3079,7 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>0.9345544053575832</v>
+        <v>0.5948143142666905</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -3131,13 +3087,13 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>1390.79682395418</v>
+        <v>8.926807634492425</v>
       </c>
       <c r="G85" t="n">
-        <v>22.14943934930855</v>
+        <v>0.03164672734327439</v>
       </c>
       <c r="H85" t="n">
-        <v>-3.569305975596037</v>
+        <v>-0.00100155611758851</v>
       </c>
     </row>
     <row r="86">
@@ -3146,7 +3102,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>h292.mtx</t>
+          <t>494_bus.mtx</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3154,9 +3110,7 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D86" t="n">
-        <v>0.06054646846778388</v>
-      </c>
+      <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr">
         <is>
           <t>Linear</t>
@@ -3165,12 +3119,8 @@
       <c r="F86" t="n">
         <v>0</v>
       </c>
-      <c r="G86" t="n">
-        <v>-0.3452356188970332</v>
-      </c>
-      <c r="H86" t="n">
-        <v>19.70159970392843</v>
-      </c>
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -3178,7 +3128,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>h292.mtx</t>
+          <t>494_bus.mtx</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3186,9 +3136,7 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D87" t="n">
-        <v>0.2358739164227963</v>
-      </c>
+      <c r="D87" t="inlineStr"/>
       <c r="E87" t="inlineStr">
         <is>
           <t>Logaritmo</t>
@@ -3197,12 +3145,8 @@
       <c r="F87" t="n">
         <v>0</v>
       </c>
-      <c r="G87" t="n">
-        <v>-10.14780599125581</v>
-      </c>
-      <c r="H87" t="n">
-        <v>40.87950552257784</v>
-      </c>
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -3210,7 +3154,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>h292.mtx</t>
+          <t>494_bus.mtx</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3218,9 +3162,7 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D88" t="n">
-        <v>0.04266563243303279</v>
-      </c>
+      <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr">
         <is>
           <t>Exponencial</t>
@@ -3229,12 +3171,8 @@
       <c r="F88" t="n">
         <v>0</v>
       </c>
-      <c r="G88" t="n">
-        <v>-0.006318065825669516</v>
-      </c>
-      <c r="H88" t="n">
-        <v>11.06234759596793</v>
-      </c>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -3242,7 +3180,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>h292.mtx</t>
+          <t>494_bus.mtx</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3250,9 +3188,7 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D89" t="n">
-        <v>0.04266563243303279</v>
-      </c>
+      <c r="D89" t="inlineStr"/>
       <c r="E89" t="inlineStr">
         <is>
           <t>Geometrico</t>
@@ -3261,12 +3197,8 @@
       <c r="F89" t="n">
         <v>0</v>
       </c>
-      <c r="G89" t="n">
-        <v>0.9937018511844836</v>
-      </c>
-      <c r="H89" t="n">
-        <v>11.06234759596793</v>
-      </c>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -3274,7 +3206,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>h292.mtx</t>
+          <t>494_bus.mtx</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3282,9 +3214,7 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D90" t="n">
-        <v>0.1945261967902213</v>
-      </c>
+      <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr">
         <is>
           <t>Potencial</t>
@@ -3293,12 +3223,8 @@
       <c r="F90" t="n">
         <v>0</v>
       </c>
-      <c r="G90" t="n">
-        <v>-0.2009070185869175</v>
-      </c>
-      <c r="H90" t="n">
-        <v>17.02560669730513</v>
-      </c>
+      <c r="G90" t="inlineStr"/>
+      <c r="H90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -3306,7 +3232,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>h292.mtx</t>
+          <t>494_bus.mtx</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3314,22 +3240,30 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D91" t="n">
-        <v>0.1563077498004442</v>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
           <t>Polinomial</t>
         </is>
       </c>
-      <c r="F91" t="n">
-        <v>33.17983626436691</v>
-      </c>
-      <c r="G91" t="n">
-        <v>-2.065861562782798</v>
-      </c>
-      <c r="H91" t="n">
-        <v>0.03740491182360359</v>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
       </c>
     </row>
     <row r="92">
@@ -3338,7 +3272,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>h292.mtx</t>
+          <t>494_bus.mtx</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3346,9 +3280,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D92" t="n">
-        <v>0.1208639325935591</v>
-      </c>
+      <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr">
         <is>
           <t>Linear</t>
@@ -3357,12 +3289,8 @@
       <c r="F92" t="n">
         <v>0</v>
       </c>
-      <c r="G92" t="n">
-        <v>-1.320827627871237</v>
-      </c>
-      <c r="H92" t="n">
-        <v>30.27104677220899</v>
-      </c>
+      <c r="G92" t="inlineStr"/>
+      <c r="H92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -3370,7 +3298,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>h292.mtx</t>
+          <t>494_bus.mtx</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3378,9 +3306,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D93" t="n">
-        <v>0.3423476533317641</v>
-      </c>
+      <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr">
         <is>
           <t>Logaritmo</t>
@@ -3389,12 +3315,8 @@
       <c r="F93" t="n">
         <v>0</v>
       </c>
-      <c r="G93" t="n">
-        <v>-18.24296999119577</v>
-      </c>
-      <c r="H93" t="n">
-        <v>55.35411670419337</v>
-      </c>
+      <c r="G93" t="inlineStr"/>
+      <c r="H93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -3402,7 +3324,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>h292.mtx</t>
+          <t>494_bus.mtx</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3410,9 +3332,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D94" t="n">
-        <v>0.1037844233913559</v>
-      </c>
+      <c r="D94" t="inlineStr"/>
       <c r="E94" t="inlineStr">
         <is>
           <t>Exponencial</t>
@@ -3421,12 +3341,8 @@
       <c r="F94" t="n">
         <v>0</v>
       </c>
-      <c r="G94" t="n">
-        <v>-0.02663577215576705</v>
-      </c>
-      <c r="H94" t="n">
-        <v>13.99254519669727</v>
-      </c>
+      <c r="G94" t="inlineStr"/>
+      <c r="H94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -3434,7 +3350,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>h292.mtx</t>
+          <t>494_bus.mtx</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3442,9 +3358,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D95" t="n">
-        <v>0.1037844233913559</v>
-      </c>
+      <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr">
         <is>
           <t>Geometrico</t>
@@ -3453,12 +3367,8 @@
       <c r="F95" t="n">
         <v>0</v>
       </c>
-      <c r="G95" t="n">
-        <v>0.9737158313628234</v>
-      </c>
-      <c r="H95" t="n">
-        <v>13.99254519669727</v>
-      </c>
+      <c r="G95" t="inlineStr"/>
+      <c r="H95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -3466,7 +3376,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>h292.mtx</t>
+          <t>494_bus.mtx</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3474,9 +3384,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D96" t="n">
-        <v>0.3087915320536542</v>
-      </c>
+      <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr">
         <is>
           <t>Potencial</t>
@@ -3485,12 +3393,8 @@
       <c r="F96" t="n">
         <v>0</v>
       </c>
-      <c r="G96" t="n">
-        <v>-0.3770474222525323</v>
-      </c>
-      <c r="H96" t="n">
-        <v>23.68643605955248</v>
-      </c>
+      <c r="G96" t="inlineStr"/>
+      <c r="H96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -3498,7 +3402,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>h292.mtx</t>
+          <t>494_bus.mtx</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3506,22 +3410,30 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D97" t="n">
-        <v>0.2920521691928787</v>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
           <t>Polinomial</t>
         </is>
       </c>
-      <c r="F97" t="n">
-        <v>56.84160758951059</v>
-      </c>
-      <c r="G97" t="n">
-        <v>-7.697762224023614</v>
-      </c>
-      <c r="H97" t="n">
-        <v>0.2657056081730156</v>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
       </c>
     </row>
     <row r="98">
@@ -3530,7 +3442,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>bcspwr03.mtx</t>
+          <t>h85.mtx</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3539,7 +3451,7 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>0.07951512074077391</v>
+        <v>0.6280816768302783</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -3550,10 +3462,10 @@
         <v>0</v>
       </c>
       <c r="G98" t="n">
-        <v>-0.1951067431376786</v>
+        <v>0.001377125402939201</v>
       </c>
       <c r="H98" t="n">
-        <v>9.778452403127579</v>
+        <v>6.691388533332892</v>
       </c>
     </row>
     <row r="99">
@@ -3562,7 +3474,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>bcspwr03.mtx</t>
+          <t>h85.mtx</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3571,7 +3483,7 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>0.2735983877967609</v>
+        <v>0.814297217800366</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -3582,10 +3494,10 @@
         <v>0</v>
       </c>
       <c r="G99" t="n">
-        <v>-4.296646601443721</v>
+        <v>0.02157074814621241</v>
       </c>
       <c r="H99" t="n">
-        <v>17.57729062029519</v>
+        <v>6.655857261175865</v>
       </c>
     </row>
     <row r="100">
@@ -3594,7 +3506,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>bcspwr03.mtx</t>
+          <t>h85.mtx</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3603,7 +3515,7 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>0.06935037387570486</v>
+        <v>0.6274001779791197</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3614,10 +3526,10 @@
         <v>0</v>
       </c>
       <c r="G100" t="n">
-        <v>-0.009683464215128307</v>
+        <v>0.0002053685450048958</v>
       </c>
       <c r="H100" t="n">
-        <v>6.429027705070445</v>
+        <v>6.691389244992517</v>
       </c>
     </row>
     <row r="101">
@@ -3626,7 +3538,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>bcspwr03.mtx</t>
+          <t>h85.mtx</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3635,7 +3547,7 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>0.06935037387570486</v>
+        <v>0.6274001779791197</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -3646,10 +3558,10 @@
         <v>0</v>
       </c>
       <c r="G101" t="n">
-        <v>0.9903632695545632</v>
+        <v>1.000205389634568</v>
       </c>
       <c r="H101" t="n">
-        <v>6.429027705070445</v>
+        <v>6.691389244992517</v>
       </c>
     </row>
     <row r="102">
@@ -3658,7 +3570,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>bcspwr03.mtx</t>
+          <t>h85.mtx</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3667,7 +3579,7 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>0.2516195345665</v>
+        <v>0.813697732040973</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -3678,10 +3590,10 @@
         <v>0</v>
       </c>
       <c r="G102" t="n">
-        <v>-0.2189797599824911</v>
+        <v>0.003217373387954841</v>
       </c>
       <c r="H102" t="n">
-        <v>9.611659479563677</v>
+        <v>6.656017221888688</v>
       </c>
     </row>
     <row r="103">
@@ -3690,7 +3602,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>bcspwr03.mtx</t>
+          <t>h85.mtx</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3699,7 +3611,7 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>0.2001666815504244</v>
+        <v>0.9069707555916999</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3707,13 +3619,13 @@
         </is>
       </c>
       <c r="F103" t="n">
-        <v>15.69208940112438</v>
+        <v>6.658504655944458</v>
       </c>
       <c r="G103" t="n">
-        <v>-1.154074904974998</v>
+        <v>0.006340729537043048</v>
       </c>
       <c r="H103" t="n">
-        <v>0.0266380044954811</v>
+        <v>-0.0001551126291907483</v>
       </c>
     </row>
     <row r="104">
@@ -3722,7 +3634,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>bcspwr03.mtx</t>
+          <t>h85.mtx</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3731,7 +3643,7 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>0.2438702448125146</v>
+        <v>0.6594176877038253</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3742,10 +3654,10 @@
         <v>0</v>
       </c>
       <c r="G104" t="n">
-        <v>-1.884643406668814</v>
+        <v>0.0008257280093627972</v>
       </c>
       <c r="H104" t="n">
-        <v>20.15627409642498</v>
+        <v>6.708785489606742</v>
       </c>
     </row>
     <row r="105">
@@ -3754,7 +3666,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>bcspwr03.mtx</t>
+          <t>h85.mtx</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3763,7 +3675,7 @@
         </is>
       </c>
       <c r="D105" t="n">
-        <v>0.4935680662741987</v>
+        <v>0.8051214258087412</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -3774,10 +3686,10 @@
         <v>0</v>
       </c>
       <c r="G105" t="n">
-        <v>-11.93435946142721</v>
+        <v>0.009502316343547052</v>
       </c>
       <c r="H105" t="n">
-        <v>27.83739849615907</v>
+        <v>6.695735493073118</v>
       </c>
     </row>
     <row r="106">
@@ -3786,7 +3698,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>bcspwr03.mtx</t>
+          <t>h85.mtx</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3795,7 +3707,7 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>0.2270469088448738</v>
+        <v>0.6591990110000472</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3806,10 +3718,10 @@
         <v>0</v>
       </c>
       <c r="G106" t="n">
-        <v>-0.09685622902927267</v>
+        <v>0.0001229545047847506</v>
       </c>
       <c r="H106" t="n">
-        <v>11.02221571317562</v>
+        <v>6.708787330937379</v>
       </c>
     </row>
     <row r="107">
@@ -3818,7 +3730,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>bcspwr03.mtx</t>
+          <t>h85.mtx</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3827,7 +3739,7 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>0.2270469088448738</v>
+        <v>0.6591990110000472</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3838,10 +3750,10 @@
         <v>0</v>
       </c>
       <c r="G107" t="n">
-        <v>0.9076864957213464</v>
+        <v>1.000122962064</v>
       </c>
       <c r="H107" t="n">
-        <v>11.02221571317562</v>
+        <v>6.708787330937379</v>
       </c>
     </row>
     <row r="108">
@@ -3850,7 +3762,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>bcspwr03.mtx</t>
+          <t>h85.mtx</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3859,7 +3771,7 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>0.4711581042726687</v>
+        <v>0.8049254128495525</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3870,10 +3782,10 @@
         <v>0</v>
       </c>
       <c r="G108" t="n">
-        <v>-0.6210533347935537</v>
+        <v>0.001414998771912366</v>
       </c>
       <c r="H108" t="n">
-        <v>16.55925513346756</v>
+        <v>6.695762472584152</v>
       </c>
     </row>
     <row r="109">
@@ -3882,7 +3794,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>bcspwr03.mtx</t>
+          <t>h85.mtx</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3891,7 +3803,7 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>0.5308208766213977</v>
+        <v>0.9275439958300997</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3899,13 +3811,13 @@
         </is>
       </c>
       <c r="F109" t="n">
-        <v>39.18805465931979</v>
+        <v>6.691713684703854</v>
       </c>
       <c r="G109" t="n">
-        <v>-10.66854212800488</v>
+        <v>0.004210654843557008</v>
       </c>
       <c r="H109" t="n">
-        <v>0.7319915601113386</v>
+        <v>-0.0001471707319214852</v>
       </c>
     </row>
     <row r="110">
@@ -3914,7 +3826,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>h85.mtx</t>
+          <t>662_bus.mtx</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3922,9 +3834,7 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D110" t="n">
-        <v>0.1055554492440328</v>
-      </c>
+      <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr">
         <is>
           <t>Linear</t>
@@ -3933,12 +3843,8 @@
       <c r="F110" t="n">
         <v>0</v>
       </c>
-      <c r="G110" t="n">
-        <v>-0.4055281690682776</v>
-      </c>
-      <c r="H110" t="n">
-        <v>14.28580124014554</v>
-      </c>
+      <c r="G110" t="inlineStr"/>
+      <c r="H110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -3946,7 +3852,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>h85.mtx</t>
+          <t>662_bus.mtx</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3954,9 +3860,7 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D111" t="n">
-        <v>0.3196106860718527</v>
-      </c>
+      <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr">
         <is>
           <t>Logaritmo</t>
@@ -3965,12 +3869,8 @@
       <c r="F111" t="n">
         <v>0</v>
       </c>
-      <c r="G111" t="n">
-        <v>-6.657877746084056</v>
-      </c>
-      <c r="H111" t="n">
-        <v>24.52752538306769</v>
-      </c>
+      <c r="G111" t="inlineStr"/>
+      <c r="H111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -3978,7 +3878,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>h85.mtx</t>
+          <t>662_bus.mtx</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3986,9 +3886,7 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D112" t="n">
-        <v>0.1015143954941921</v>
-      </c>
+      <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr">
         <is>
           <t>Exponencial</t>
@@ -3997,12 +3895,8 @@
       <c r="F112" t="n">
         <v>0</v>
       </c>
-      <c r="G112" t="n">
-        <v>-0.01669721334682383</v>
-      </c>
-      <c r="H112" t="n">
-        <v>9.172071217406748</v>
-      </c>
+      <c r="G112" t="inlineStr"/>
+      <c r="H112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -4010,7 +3904,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>h85.mtx</t>
+          <t>662_bus.mtx</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -4018,9 +3912,7 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D113" t="n">
-        <v>0.1015143954941921</v>
-      </c>
+      <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr">
         <is>
           <t>Geometrico</t>
@@ -4029,12 +3921,8 @@
       <c r="F113" t="n">
         <v>0</v>
       </c>
-      <c r="G113" t="n">
-        <v>0.9834414124925077</v>
-      </c>
-      <c r="H113" t="n">
-        <v>9.172071217406748</v>
-      </c>
+      <c r="G113" t="inlineStr"/>
+      <c r="H113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -4042,7 +3930,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>h85.mtx</t>
+          <t>662_bus.mtx</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -4050,9 +3938,7 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D114" t="n">
-        <v>0.3118101372339335</v>
-      </c>
+      <c r="D114" t="inlineStr"/>
       <c r="E114" t="inlineStr">
         <is>
           <t>Potencial</t>
@@ -4061,12 +3947,8 @@
       <c r="F114" t="n">
         <v>0</v>
       </c>
-      <c r="G114" t="n">
-        <v>-0.2761021370309458</v>
-      </c>
-      <c r="H114" t="n">
-        <v>14.04923379891252</v>
-      </c>
+      <c r="G114" t="inlineStr"/>
+      <c r="H114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -4074,7 +3956,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>h85.mtx</t>
+          <t>662_bus.mtx</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -4082,22 +3964,30 @@
           <t>MP</t>
         </is>
       </c>
-      <c r="D115" t="n">
-        <v>0.2582944364245717</v>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
           <t>Polinomial</t>
         </is>
       </c>
-      <c r="F115" t="n">
-        <v>23.78172143203886</v>
-      </c>
-      <c r="G115" t="n">
-        <v>-2.370201312218621</v>
-      </c>
-      <c r="H115" t="n">
-        <v>0.0701668979696551</v>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
       </c>
     </row>
     <row r="116">
@@ -4106,7 +3996,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>h85.mtx</t>
+          <t>662_bus.mtx</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -4114,9 +4004,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D116" t="n">
-        <v>0.1562486681291495</v>
-      </c>
+      <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr">
         <is>
           <t>Linear</t>
@@ -4125,12 +4013,8 @@
       <c r="F116" t="n">
         <v>0</v>
       </c>
-      <c r="G116" t="n">
-        <v>-0.8984253232786571</v>
-      </c>
-      <c r="H116" t="n">
-        <v>18.09676691630873</v>
-      </c>
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -4138,7 +4022,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>h85.mtx</t>
+          <t>662_bus.mtx</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -4146,9 +4030,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D117" t="n">
-        <v>0.3932367670763982</v>
-      </c>
+      <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr">
         <is>
           <t>Logaritmo</t>
@@ -4157,12 +4039,8 @@
       <c r="F117" t="n">
         <v>0</v>
       </c>
-      <c r="G117" t="n">
-        <v>-9.489308265948354</v>
-      </c>
-      <c r="H117" t="n">
-        <v>28.74881518157584</v>
-      </c>
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -4170,7 +4048,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>h85.mtx</t>
+          <t>662_bus.mtx</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -4178,9 +4056,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D118" t="n">
-        <v>0.1520289748408564</v>
-      </c>
+      <c r="D118" t="inlineStr"/>
       <c r="E118" t="inlineStr">
         <is>
           <t>Exponencial</t>
@@ -4189,12 +4065,8 @@
       <c r="F118" t="n">
         <v>0</v>
       </c>
-      <c r="G118" t="n">
-        <v>-0.03720779120574044</v>
-      </c>
-      <c r="H118" t="n">
-        <v>10.76063033446828</v>
-      </c>
+      <c r="G118" t="inlineStr"/>
+      <c r="H118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -4202,7 +4074,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>h85.mtx</t>
+          <t>662_bus.mtx</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4210,9 +4082,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D119" t="n">
-        <v>0.1520289748408564</v>
-      </c>
+      <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr">
         <is>
           <t>Geometrico</t>
@@ -4221,12 +4091,8 @@
       <c r="F119" t="n">
         <v>0</v>
       </c>
-      <c r="G119" t="n">
-        <v>0.9634759127259166</v>
-      </c>
-      <c r="H119" t="n">
-        <v>10.76063033446828</v>
-      </c>
+      <c r="G119" t="inlineStr"/>
+      <c r="H119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -4234,7 +4100,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>h85.mtx</t>
+          <t>662_bus.mtx</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4242,9 +4108,7 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D120" t="n">
-        <v>0.3859919703620887</v>
-      </c>
+      <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr">
         <is>
           <t>Potencial</t>
@@ -4253,12 +4117,8 @@
       <c r="F120" t="n">
         <v>0</v>
       </c>
-      <c r="G120" t="n">
-        <v>-0.3947239837301336</v>
-      </c>
-      <c r="H120" t="n">
-        <v>16.78591004710673</v>
-      </c>
+      <c r="G120" t="inlineStr"/>
+      <c r="H120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -4266,7 +4126,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>h85.mtx</t>
+          <t>662_bus.mtx</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -4274,22 +4134,30 @@
           <t>MP_Aitken</t>
         </is>
       </c>
-      <c r="D121" t="n">
-        <v>0.3655760872045868</v>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
           <t>Polinomial</t>
         </is>
       </c>
-      <c r="F121" t="n">
-        <v>32.35579316662525</v>
-      </c>
-      <c r="G121" t="n">
-        <v>-5.176133198373615</v>
-      </c>
-      <c r="H121" t="n">
-        <v>0.2251425197418399</v>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>erro</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>